<commit_message>
Feat: successfully parsing into Polymerisation objects and adding to DB
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/433420f6ee06d484/Documents/Imperial/project/roppy/db_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Arch\home\rmrr\roppy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="257" documentId="8_{54D75658-8D3E-4820-80D9-E43200F7499D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3379CD96-18AB-4241-9496-FAD24A5AE231}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BB30DA-2D53-491F-A654-A7AC0D322D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45020" yWindow="2610" windowWidth="27020" windowHeight="16990" xr2:uid="{A2D599AD-951E-4FCA-918A-61913270540F}"/>
+    <workbookView xWindow="38630" yWindow="5350" windowWidth="27020" windowHeight="12530" activeTab="1" xr2:uid="{A2D599AD-951E-4FCA-918A-61913270540F}"/>
   </bookViews>
   <sheets>
-    <sheet name="annotated" sheetId="1" r:id="rId1"/>
+    <sheet name="draft" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="223">
   <si>
     <t>Monomer</t>
   </si>
@@ -387,13 +388,331 @@
   </si>
   <si>
     <t>MonomerSummaryBrief.has_calc</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
+    <t>pressure</t>
+  </si>
+  <si>
+    <t>solvent</t>
+  </si>
+  <si>
+    <t>solvent_conc</t>
+  </si>
+  <si>
+    <t>monomer_state</t>
+  </si>
+  <si>
+    <t>polymer_state</t>
+  </si>
+  <si>
+    <t>ceiling_temperature</t>
+  </si>
+  <si>
+    <t>solvent_model</t>
+  </si>
+  <si>
+    <t>C1COC1=O</t>
+  </si>
+  <si>
+    <t>CC1(COC1=O)C</t>
+  </si>
+  <si>
+    <t>C1CC(=O)OC1</t>
+  </si>
+  <si>
+    <t>C=C1CCOC1=O</t>
+  </si>
+  <si>
+    <t>O=C1CCCO1</t>
+  </si>
+  <si>
+    <t>O=C1OCCC1</t>
+  </si>
+  <si>
+    <t>O=C1NCCO1</t>
+  </si>
+  <si>
+    <t>O=C1CCCC(CC)O1</t>
+  </si>
+  <si>
+    <t>O=C1CCCC(C)O1</t>
+  </si>
+  <si>
+    <t>O=C1CCC(C)CO1</t>
+  </si>
+  <si>
+    <t>O=C1CC(C)CCO1</t>
+  </si>
+  <si>
+    <t>O=C1C(CCCCCCCCC)CCCO1</t>
+  </si>
+  <si>
+    <t>O=C1C(C)CCCO1</t>
+  </si>
+  <si>
+    <t>O=C1C(C)OCCO1</t>
+  </si>
+  <si>
+    <t>O=C1CCCC(CCC)O1</t>
+  </si>
+  <si>
+    <t>O=C(O[C@H]1C)[C@H](C)OC1=O</t>
+  </si>
+  <si>
+    <t>O=C(OCc1ccccc1)C2CC=CC2</t>
+  </si>
+  <si>
+    <t>COC(=O)C1CCC(=O)OC1</t>
+  </si>
+  <si>
+    <t>CCCCCCCCCC1CCCC(O1)=O</t>
+  </si>
+  <si>
+    <t>CCCCCCCCCC1CCCC(=O)O1</t>
+  </si>
+  <si>
+    <t>O=C1C(CCCCC)CCCO1</t>
+  </si>
+  <si>
+    <t>O=C1CCCC(CCCC)O1</t>
+  </si>
+  <si>
+    <t>O=C1CCCC(CCCCCCC)O1</t>
+  </si>
+  <si>
+    <t>O=C1CCCC(CCCCCC)O1</t>
+  </si>
+  <si>
+    <t>CCCCCCCC1CCCC(=O)O1</t>
+  </si>
+  <si>
+    <t>O=C1CCCC(O1)CCCCC</t>
+  </si>
+  <si>
+    <t>O=C1CCCCO1</t>
+  </si>
+  <si>
+    <t>O=C1CCOC(C)O1</t>
+  </si>
+  <si>
+    <t>O=C1COCC(C)O1</t>
+  </si>
+  <si>
+    <t>O=C1COCCO1</t>
+  </si>
+  <si>
+    <t>O=C1CSCCS1</t>
+  </si>
+  <si>
+    <t>O=C1NCCCO1</t>
+  </si>
+  <si>
+    <t>O=C1OCCCO1</t>
+  </si>
+  <si>
+    <t>O=C1OCCOC1</t>
+  </si>
+  <si>
+    <t>O=C1SCCSC1</t>
+  </si>
+  <si>
+    <t>O=C1SCCSC1(C)C</t>
+  </si>
+  <si>
+    <t>O=C1SCCSC1C</t>
+  </si>
+  <si>
+    <t>O=C1CCCC(CCCCC)O1</t>
+  </si>
+  <si>
+    <t>CCCCCCC1CCCC(O1)=O</t>
+  </si>
+  <si>
+    <t>O=C(OC1)COC1=O</t>
+  </si>
+  <si>
+    <t>CCCCCC1CCCC(O1)=O</t>
+  </si>
+  <si>
+    <t>CC(CCO1)CC1=O</t>
+  </si>
+  <si>
+    <t>CC1CCCC(=O)O1</t>
+  </si>
+  <si>
+    <t>C1CC2CCC1C(=O)O2</t>
+  </si>
+  <si>
+    <t>C=C1CCCOC1=O</t>
+  </si>
+  <si>
+    <t>CCCCCCC1CCCC(=O)O1</t>
+  </si>
+  <si>
+    <t>C=CCOCC1(CC)COC(=O)OC1</t>
+  </si>
+  <si>
+    <t>CC1CCCOC1=O</t>
+  </si>
+  <si>
+    <t>CC(=O)OC1CC(=O)OC(C)C1</t>
+  </si>
+  <si>
+    <t>CC(C)(C)OC(=O)N1CCOC(=O)C1</t>
+  </si>
+  <si>
+    <t>CC1CCC(=O)OC1</t>
+  </si>
+  <si>
+    <t>CC1CC(OC(C)=O)CC(O1)=O</t>
+  </si>
+  <si>
+    <t>CC1(SCCSC1=O)C</t>
+  </si>
+  <si>
+    <t>CC1(C)SCCSC1=O</t>
+  </si>
+  <si>
+    <t>CC1(C)COC(=O)OC1</t>
+  </si>
+  <si>
+    <t>CC(C(OC1C)=O)OC1=O</t>
+  </si>
+  <si>
+    <t>CC1CCOC(=O)C1</t>
+  </si>
+  <si>
+    <t>CC1CCCC(O1)=O</t>
+  </si>
+  <si>
+    <t>CC1OC(=O)C(C)OC1=O</t>
+  </si>
+  <si>
+    <t>CCCCCC1CCCC(=O)O1</t>
+  </si>
+  <si>
+    <t>CCCCC1CCCC(O1)=O</t>
+  </si>
+  <si>
+    <t>CCCCC1CCCC(=O)O1</t>
+  </si>
+  <si>
+    <t>CCCC1CCCC(O1)=O</t>
+  </si>
+  <si>
+    <t>CCCC1CCCC(=O)O1</t>
+  </si>
+  <si>
+    <t>CC1CCOC(C1)=O</t>
+  </si>
+  <si>
+    <t>CCC1CCCC(O1)=O</t>
+  </si>
+  <si>
+    <t>CCC1CCCC(=O)O1</t>
+  </si>
+  <si>
+    <t>CC(C)C1CC(=O)OC(C)C1</t>
+  </si>
+  <si>
+    <t>CC2(c1ccccc1)COC(=O)OC2</t>
+  </si>
+  <si>
+    <t>CC1SCCSC1=O</t>
+  </si>
+  <si>
+    <t>CC1OCCOC1=O</t>
+  </si>
+  <si>
+    <t>CC1OCCC(=O)O1</t>
+  </si>
+  <si>
+    <t>CCC1(CC)COC(=O)OC1</t>
+  </si>
+  <si>
+    <t>CC2(C)Oc1ccccc1COC2=O</t>
+  </si>
+  <si>
+    <t>O=C1CC(C(C)C)CCC(C)O1</t>
+  </si>
+  <si>
+    <t>O=C1CCCCCO1</t>
+  </si>
+  <si>
+    <t>CC1CCC(C(C)C)OC(=O)C1</t>
+  </si>
+  <si>
+    <t>O=C1[C@@H](C(C)C)CC[C@@H](C)CO1</t>
+  </si>
+  <si>
+    <t>CC1CCC(OC(C1)=O)C(C)C</t>
+  </si>
+  <si>
+    <t>O=C1NCCCCO1</t>
+  </si>
+  <si>
+    <t>O=C1OCCCCCC1</t>
+  </si>
+  <si>
+    <t>S=C1CCCCCC(O1)=O</t>
+  </si>
+  <si>
+    <t>O=C1CCCCCCO1</t>
+  </si>
+  <si>
+    <t>O=C1OCCCCCCC1</t>
+  </si>
+  <si>
+    <t>O=C1CCCCCCCCO1</t>
+  </si>
+  <si>
+    <t>O=C1CCCCCCCCCO1</t>
+  </si>
+  <si>
+    <t>O=C1CCCCCCCCCCO1</t>
+  </si>
+  <si>
+    <t>O=C1CCCCCCCCCCCO1</t>
+  </si>
+  <si>
+    <t>O=C1CCCCCCCCCCCCO1</t>
+  </si>
+  <si>
+    <t>O=C1CCCCCCCCCCCCCO1</t>
+  </si>
+  <si>
+    <t>O=C1CCCCCCCCCCCCCCO1</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>he</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>initiator_smiles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +727,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -454,13 +779,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,10 +807,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -806,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C739B02-EDBE-4575-91DA-57112997C50A}">
   <dimension ref="A1:AK48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1404,4 +1726,1736 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84990456-B1AB-4E0C-A4B4-A3558CADED39}">
+  <dimension ref="A1:V105"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="28" width="16.578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>-82.3</v>
+      </c>
+      <c r="R2" s="6">
+        <v>-74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>-84</v>
+      </c>
+      <c r="R3" s="6">
+        <v>-74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>5</v>
+      </c>
+      <c r="R4" s="6">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="Q5" s="6">
+        <v>-5.9</v>
+      </c>
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" s="6">
+        <v>200</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>5</v>
+      </c>
+      <c r="R6" s="6">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="J7" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="Q7" s="6">
+        <v>-5.4</v>
+      </c>
+      <c r="R7" s="6">
+        <v>-39.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="Q8" s="6">
+        <v>-1.7</v>
+      </c>
+      <c r="R8" s="6"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="J9" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>-16.399999999999999</v>
+      </c>
+      <c r="R9" s="6">
+        <v>-55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="J10" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>-13.8</v>
+      </c>
+      <c r="R10" s="6">
+        <v>-41.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" s="6">
+        <v>300.14999999999998</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>-15.8</v>
+      </c>
+      <c r="R11" s="6">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="6">
+        <v>419.15</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>-14.3</v>
+      </c>
+      <c r="R12" s="6">
+        <v>-28.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E13" s="6">
+        <v>300.14999999999998</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>-16.8</v>
+      </c>
+      <c r="R13" s="6">
+        <v>-55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="J14" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>-13</v>
+      </c>
+      <c r="R14" s="6">
+        <v>-34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="J15" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>-9.9</v>
+      </c>
+      <c r="R15" s="6">
+        <v>-39.200000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="J16" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>-18.5</v>
+      </c>
+      <c r="R16" s="6">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="J17" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>-23.9</v>
+      </c>
+      <c r="R17" s="6">
+        <v>-43.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="Q18" s="6">
+        <v>-21.02</v>
+      </c>
+      <c r="R18" s="6"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="Q19" s="6">
+        <v>-15.2</v>
+      </c>
+      <c r="R19" s="6"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="Q20" s="6">
+        <v>-16.8</v>
+      </c>
+      <c r="R20" s="6"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="Q21" s="6">
+        <v>-16.8</v>
+      </c>
+      <c r="R21" s="6"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="J22" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q22" s="6">
+        <v>-17.100000000000001</v>
+      </c>
+      <c r="R22" s="6">
+        <v>-54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E23" s="6">
+        <v>300.14999999999998</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q23" s="6">
+        <v>-17</v>
+      </c>
+      <c r="R23" s="6">
+        <v>-55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E24" s="6">
+        <v>300.14999999999998</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q24" s="6">
+        <v>-18.7</v>
+      </c>
+      <c r="R24" s="6">
+        <v>-59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" s="6">
+        <v>300.14999999999998</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q25" s="6">
+        <v>-18.399999999999999</v>
+      </c>
+      <c r="R25" s="6">
+        <v>-58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="Q26" s="6">
+        <v>-18.7</v>
+      </c>
+      <c r="R26" s="6"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E27" s="6">
+        <v>372.15</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q27" s="6">
+        <v>-20</v>
+      </c>
+      <c r="R27" s="6">
+        <v>-48.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E28" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="Q28" s="6">
+        <v>-10.5</v>
+      </c>
+      <c r="R28" s="6">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E29" s="6">
+        <v>194.15</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q29" s="6">
+        <v>-10.9</v>
+      </c>
+      <c r="R29" s="6">
+        <v>-41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="J30" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q30" s="6">
+        <v>-11.6</v>
+      </c>
+      <c r="R30" s="6">
+        <v>-52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="Q31" s="6">
+        <v>-14.1</v>
+      </c>
+      <c r="R31" s="6"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="Q32" s="6">
+        <v>-9.5</v>
+      </c>
+      <c r="R32" s="6"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="Q33" s="6">
+        <v>-18</v>
+      </c>
+      <c r="R33" s="6"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="Q34" s="6">
+        <v>-26</v>
+      </c>
+      <c r="R34" s="6"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E35" s="6">
+        <v>373</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q35" s="6">
+        <v>-13.8</v>
+      </c>
+      <c r="R35" s="6">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E36" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q36" s="6">
+        <v>-9.5</v>
+      </c>
+      <c r="R36" s="6">
+        <v>-30.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="E37" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q37" s="6">
+        <v>-19.3</v>
+      </c>
+      <c r="R37" s="6">
+        <v>-58.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E38" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q38" s="6">
+        <v>-10.199999999999999</v>
+      </c>
+      <c r="R38" s="6">
+        <v>-39.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E39" s="6">
+        <v>300.14999999999998</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q39" s="6">
+        <v>-18</v>
+      </c>
+      <c r="R39" s="6">
+        <v>-57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="Q40" s="6">
+        <v>-18.399999999999999</v>
+      </c>
+      <c r="R40" s="6"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E41" s="6">
+        <v>550</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q41" s="6">
+        <v>-15.7</v>
+      </c>
+      <c r="R41" s="6">
+        <v>-8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="Q42" s="6">
+        <v>-18</v>
+      </c>
+      <c r="R42" s="6"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E43" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="Q43" s="6">
+        <v>-13.8</v>
+      </c>
+      <c r="R43" s="6">
+        <v>-46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E44" s="6"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6"/>
+      <c r="Q44" s="6">
+        <v>-13.8</v>
+      </c>
+      <c r="R44" s="6"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E45" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q45" s="6">
+        <v>-35</v>
+      </c>
+      <c r="R45" s="6">
+        <v>-76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="E46" s="6"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6"/>
+      <c r="Q46" s="6">
+        <v>-16.5</v>
+      </c>
+      <c r="R46" s="6"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="Q47" s="6">
+        <v>-18.399999999999999</v>
+      </c>
+      <c r="R47" s="6"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+      <c r="Q48" s="6">
+        <v>-22</v>
+      </c>
+      <c r="R48" s="6"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E49" s="6"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="6"/>
+      <c r="Q49" s="6">
+        <v>-13</v>
+      </c>
+      <c r="R49" s="6"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E50" s="6"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="6"/>
+      <c r="Q50" s="6">
+        <v>-25</v>
+      </c>
+      <c r="R50" s="6"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="Q51" s="6">
+        <v>-19.63</v>
+      </c>
+      <c r="R51" s="6"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="Q52" s="6">
+        <v>-15.8</v>
+      </c>
+      <c r="R52" s="6"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E53" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="Q53" s="6">
+        <v>-25</v>
+      </c>
+      <c r="R53" s="6">
+        <v>-10.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="Q54" s="6">
+        <v>-19.3</v>
+      </c>
+      <c r="R54" s="6"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E55" s="6"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6"/>
+      <c r="Q55" s="6">
+        <v>-19.3</v>
+      </c>
+      <c r="R55" s="6"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E56" s="6"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="6"/>
+      <c r="Q56" s="6">
+        <v>-21</v>
+      </c>
+      <c r="R56" s="6"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="E57" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J57" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q57" s="6">
+        <v>-22.9</v>
+      </c>
+      <c r="R57" s="6">
+        <v>-41.1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E58" s="6"/>
+      <c r="J58" s="6"/>
+      <c r="K58" s="6"/>
+      <c r="Q58" s="6">
+        <v>-13.8</v>
+      </c>
+      <c r="R58" s="6"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E59" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J59" s="6"/>
+      <c r="K59" s="6"/>
+      <c r="Q59" s="6">
+        <v>-13.8</v>
+      </c>
+      <c r="R59" s="6">
+        <v>-41.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E60" s="6"/>
+      <c r="J60" s="6"/>
+      <c r="K60" s="6"/>
+      <c r="Q60" s="6">
+        <v>-23.9</v>
+      </c>
+      <c r="R60" s="6"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E61" s="6"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
+      <c r="Q61" s="6">
+        <v>-17.100000000000001</v>
+      </c>
+      <c r="R61" s="6"/>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="Q62" s="6">
+        <v>-17</v>
+      </c>
+      <c r="R62" s="6"/>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="Q63" s="6">
+        <v>-17</v>
+      </c>
+      <c r="R63" s="6"/>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="Q64" s="6">
+        <v>-18.5</v>
+      </c>
+      <c r="R64" s="6"/>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="Q65" s="6">
+        <v>-18.5</v>
+      </c>
+      <c r="R65" s="6"/>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E66" s="6"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="Q66" s="6">
+        <v>-13.8</v>
+      </c>
+      <c r="R66" s="6"/>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="Q67" s="6">
+        <v>-16.399999999999999</v>
+      </c>
+      <c r="R67" s="6"/>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="Q68" s="6">
+        <v>-16.399999999999999</v>
+      </c>
+      <c r="R68" s="6"/>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E69" s="6"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="Q69" s="6">
+        <v>-16.8</v>
+      </c>
+      <c r="R69" s="6"/>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E70" s="6"/>
+      <c r="J70" s="6"/>
+      <c r="K70" s="6"/>
+      <c r="Q70" s="6">
+        <v>-16</v>
+      </c>
+      <c r="R70" s="6"/>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E71" s="6"/>
+      <c r="J71" s="6"/>
+      <c r="K71" s="6"/>
+      <c r="Q71" s="6">
+        <v>-10.199999999999999</v>
+      </c>
+      <c r="R71" s="6"/>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E72" s="6"/>
+      <c r="J72" s="6"/>
+      <c r="K72" s="6"/>
+      <c r="Q72" s="6">
+        <v>-9.85</v>
+      </c>
+      <c r="R72" s="6"/>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E73" s="6"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="Q73" s="6">
+        <v>-11.6</v>
+      </c>
+      <c r="R73" s="6"/>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="Q74" s="6">
+        <v>-18</v>
+      </c>
+      <c r="R74" s="6"/>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="E75" s="6"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="6"/>
+      <c r="Q75" s="6">
+        <v>-27.3</v>
+      </c>
+      <c r="R75" s="6"/>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E76" s="6"/>
+      <c r="J76" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K76" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q76" s="6">
+        <v>-16.8</v>
+      </c>
+      <c r="R76" s="6">
+        <v>-27.4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="E77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="Q77" s="6">
+        <v>-14</v>
+      </c>
+      <c r="R77" s="6"/>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="E78" s="6"/>
+      <c r="J78" s="6"/>
+      <c r="K78" s="6"/>
+      <c r="Q78" s="6">
+        <v>-16.8</v>
+      </c>
+      <c r="R78" s="6"/>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E79" s="6">
+        <v>478.15</v>
+      </c>
+      <c r="J79" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="K79" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q79" s="6">
+        <v>-18.600000000000001</v>
+      </c>
+      <c r="R79" s="6">
+        <v>-33.1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="E80" s="6"/>
+      <c r="J80" s="6"/>
+      <c r="K80" s="6"/>
+      <c r="Q80" s="6">
+        <v>-16.8</v>
+      </c>
+      <c r="R80" s="6"/>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="E81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="Q81" s="6">
+        <v>-40</v>
+      </c>
+      <c r="R81" s="6"/>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="E82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="Q82" s="6">
+        <v>-19.25</v>
+      </c>
+      <c r="R82" s="6"/>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="E83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="Q83" s="6">
+        <v>-5.14</v>
+      </c>
+      <c r="R83" s="6">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="E84" s="6"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="Q84" s="6">
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="R84" s="6">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E85" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J85" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K85" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q85" s="6">
+        <v>-19</v>
+      </c>
+      <c r="R85" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E86" s="6">
+        <v>400</v>
+      </c>
+      <c r="J86" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K86" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q86" s="6">
+        <v>-22</v>
+      </c>
+      <c r="R86" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="E87" s="6">
+        <v>400</v>
+      </c>
+      <c r="J87" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K87" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q87" s="6">
+        <v>-24</v>
+      </c>
+      <c r="R87" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E88" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J88" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K88" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q88" s="6">
+        <v>-28</v>
+      </c>
+      <c r="R88" s="6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E89" s="6">
+        <v>400</v>
+      </c>
+      <c r="J89" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K89" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q89" s="6">
+        <v>-19</v>
+      </c>
+      <c r="R89" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E90" s="6">
+        <v>430</v>
+      </c>
+      <c r="J90" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K90" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q90" s="6">
+        <v>-8</v>
+      </c>
+      <c r="R90" s="6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="E91" s="6">
+        <v>400</v>
+      </c>
+      <c r="J91" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K91" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q91" s="6">
+        <v>-2</v>
+      </c>
+      <c r="R91" s="6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E92" s="6">
+        <v>200</v>
+      </c>
+      <c r="J92" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="K92" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q92" s="6">
+        <v>-12</v>
+      </c>
+      <c r="R92" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E93" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J93" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K93" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q93" s="6">
+        <v>-82.3</v>
+      </c>
+      <c r="R93" s="6">
+        <v>-74</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E94" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J94" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K94" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q94" s="6">
+        <v>5</v>
+      </c>
+      <c r="R94" s="6">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E95" s="6">
+        <v>300.14999999999998</v>
+      </c>
+      <c r="J95" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K95" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q95" s="6">
+        <v>-15.8</v>
+      </c>
+      <c r="R95" s="6">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="E96" s="6"/>
+      <c r="J96" s="6"/>
+      <c r="K96" s="6"/>
+      <c r="Q96" s="6">
+        <v>-14</v>
+      </c>
+      <c r="R96" s="6"/>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="E97" s="6"/>
+      <c r="J97" s="6"/>
+      <c r="K97" s="6"/>
+      <c r="Q97" s="6">
+        <v>-19.25</v>
+      </c>
+      <c r="R97" s="6"/>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E98" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J98" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K98" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q98" s="6">
+        <v>-19</v>
+      </c>
+      <c r="R98" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E99" s="6">
+        <v>400</v>
+      </c>
+      <c r="J99" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K99" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q99" s="6">
+        <v>-22</v>
+      </c>
+      <c r="R99" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="E100" s="6">
+        <v>400</v>
+      </c>
+      <c r="J100" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K100" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q100" s="6">
+        <v>-24</v>
+      </c>
+      <c r="R100" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E101" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="J101" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K101" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q101" s="6">
+        <v>-28</v>
+      </c>
+      <c r="R101" s="6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E102" s="6">
+        <v>400</v>
+      </c>
+      <c r="J102" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K102" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q102" s="6">
+        <v>-19</v>
+      </c>
+      <c r="R102" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E103" s="6">
+        <v>430</v>
+      </c>
+      <c r="J103" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K103" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q103" s="6">
+        <v>-8</v>
+      </c>
+      <c r="R103" s="6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="E104" s="6">
+        <v>400</v>
+      </c>
+      <c r="J104" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K104" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q104" s="6">
+        <v>-2</v>
+      </c>
+      <c r="R104" s="6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E105" s="6">
+        <v>200</v>
+      </c>
+      <c r="J105" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="K105" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q105" s="6">
+        <v>-12</v>
+      </c>
+      <c r="R105" s="6">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>